<commit_message>
Work on the input format for the Outstation Patcher.
</commit_message>
<xml_diff>
--- a/EdcPatcher/excel-sample/EDC_Worklist_Sample.xlsx
+++ b/EdcPatcher/excel-sample/EDC_Worklist_Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\work\asset-patch\EdcPatcher\excel-sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D615B46-A442-45C2-939B-E7D23E312C4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD55351F-B74F-4C96-BC28-DBE56B607FC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F9EA631D-0435-45C1-B7CC-C2C1FD7F9DA1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="102">
   <si>
     <t>NGR</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>SYS01</t>
+  </si>
+  <si>
+    <t>Zzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -710,9 +713,9 @@
   <sheetPr transitionEvaluation="1"/>
   <dimension ref="A1:AL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,6 +971,9 @@
       <c r="AK2" t="s">
         <v>57</v>
       </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1084,6 +1090,9 @@
       <c r="AK4" t="s">
         <v>57</v>
       </c>
+      <c r="AL4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1254,6 +1263,9 @@
       <c r="AK6" t="s">
         <v>57</v>
       </c>
+      <c r="AL6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1539,6 +1551,9 @@
       <c r="AK10" t="s">
         <v>57</v>
       </c>
+      <c r="AL10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1648,6 +1663,9 @@
       </c>
       <c r="AK11" t="s">
         <v>57</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>